<commit_message>
05.10.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/Others/Allocation Sheet 2.xlsx
+++ b/Others/Allocation Sheet 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho Corporation\Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB40576E-0A7C-496F-B65F-84B554F185D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068455B1-5C24-427D-9476-2E3DA23285CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,7 +445,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Md Kamrul Hasan</t>
+    <t>Md Muradur Rahman</t>
   </si>
 </sst>
 </file>
@@ -928,6 +928,81 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="11" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -940,73 +1015,43 @@
     <xf numFmtId="49" fontId="11" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1020,51 +1065,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4011,8 +4011,8 @@
   </sheetPr>
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4034,59 +4034,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
     </row>
     <row r="3" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="72"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
-      <c r="J3" s="98" t="s">
+      <c r="J3" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="K3" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
@@ -4864,13 +4864,13 @@
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
-      <c r="H36" s="74" t="s">
+      <c r="H36" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="74"/>
+      <c r="I36" s="54"/>
       <c r="J36" s="38"/>
-      <c r="K36" s="74"/>
-      <c r="L36" s="74"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
       <c r="M36" s="41"/>
     </row>
     <row r="37" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4885,12 +4885,12 @@
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="54"/>
     </row>
     <row r="38" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="45" t="s">
@@ -4904,14 +4904,14 @@
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
-      <c r="H38" s="76" t="s">
+      <c r="H38" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="76"/>
-      <c r="J38" s="76"/>
-      <c r="K38" s="76"/>
-      <c r="L38" s="76"/>
-      <c r="M38" s="77"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="56"/>
     </row>
     <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
@@ -4931,10 +4931,10 @@
       <c r="I39" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="74"/>
-      <c r="K39" s="74"/>
-      <c r="L39" s="74"/>
-      <c r="M39" s="78"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="54"/>
+      <c r="L39" s="54"/>
+      <c r="M39" s="57"/>
     </row>
     <row r="40" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="45" t="s">
@@ -4955,7 +4955,7 @@
       <c r="J40" s="38"/>
       <c r="K40" s="38"/>
       <c r="L40" s="38"/>
-      <c r="M40" s="78"/>
+      <c r="M40" s="57"/>
     </row>
     <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="45" t="s">
@@ -4976,7 +4976,7 @@
       <c r="J41" s="38"/>
       <c r="K41" s="38"/>
       <c r="L41" s="38"/>
-      <c r="M41" s="78"/>
+      <c r="M41" s="57"/>
     </row>
     <row r="42" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="45" t="s">
@@ -4997,7 +4997,7 @@
       <c r="J42" s="38"/>
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
-      <c r="M42" s="78"/>
+      <c r="M42" s="57"/>
     </row>
     <row r="43" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="45" t="s">
@@ -5018,7 +5018,7 @@
       <c r="J43" s="38"/>
       <c r="K43" s="38"/>
       <c r="L43" s="38"/>
-      <c r="M43" s="78"/>
+      <c r="M43" s="57"/>
     </row>
     <row r="44" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
@@ -5039,7 +5039,7 @@
       <c r="J44" s="38"/>
       <c r="K44" s="38"/>
       <c r="L44" s="38"/>
-      <c r="M44" s="78"/>
+      <c r="M44" s="57"/>
     </row>
     <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="45" t="s">
@@ -5060,7 +5060,7 @@
       <c r="J45" s="38"/>
       <c r="K45" s="38"/>
       <c r="L45" s="38"/>
-      <c r="M45" s="78"/>
+      <c r="M45" s="57"/>
     </row>
     <row r="46" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="45"/>
@@ -5077,7 +5077,7 @@
       <c r="J46" s="38"/>
       <c r="K46" s="38"/>
       <c r="L46" s="38"/>
-      <c r="M46" s="78"/>
+      <c r="M46" s="57"/>
     </row>
     <row r="47" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="45"/>
@@ -5094,7 +5094,7 @@
       <c r="J47" s="38"/>
       <c r="K47" s="38"/>
       <c r="L47" s="38"/>
-      <c r="M47" s="78"/>
+      <c r="M47" s="57"/>
     </row>
     <row r="48" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="44"/>
@@ -5111,43 +5111,43 @@
       <c r="J48" s="38"/>
       <c r="K48" s="38"/>
       <c r="L48" s="38"/>
-      <c r="M48" s="79"/>
+      <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="54"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="57" t="s">
+      <c r="B49" s="79"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="E49" s="57"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="57"/>
-      <c r="I49" s="57"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
       <c r="J49" s="32"/>
-      <c r="K49" s="59" t="s">
+      <c r="K49" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="L49" s="59"/>
-      <c r="M49" s="60"/>
+      <c r="L49" s="66"/>
+      <c r="M49" s="67"/>
     </row>
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="55"/>
-      <c r="B50" s="56"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
+      <c r="A50" s="80"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="65"/>
+      <c r="H50" s="65"/>
+      <c r="I50" s="65"/>
       <c r="J50" s="33"/>
-      <c r="K50" s="61"/>
-      <c r="L50" s="61"/>
-      <c r="M50" s="62"/>
+      <c r="K50" s="68"/>
+      <c r="L50" s="68"/>
+      <c r="M50" s="69"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="29"/>
@@ -5165,25 +5165,25 @@
       <c r="M51" s="30"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="63" t="s">
+      <c r="A52" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="63"/>
+      <c r="B52" s="70"/>
       <c r="C52" s="35"/>
       <c r="D52" s="29"/>
       <c r="E52" s="29"/>
-      <c r="F52" s="65" t="s">
+      <c r="F52" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="G52" s="66"/>
-      <c r="H52" s="67"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="74"/>
       <c r="I52" s="29"/>
       <c r="J52" s="35"/>
-      <c r="K52" s="64" t="s">
+      <c r="K52" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="L52" s="64"/>
-      <c r="M52" s="64"/>
+      <c r="L52" s="71"/>
+      <c r="M52" s="71"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="34"/>
@@ -5191,9 +5191,9 @@
       <c r="C53" s="35"/>
       <c r="D53" s="29"/>
       <c r="E53" s="29"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="69"/>
-      <c r="H53" s="70"/>
+      <c r="F53" s="75"/>
+      <c r="G53" s="76"/>
+      <c r="H53" s="77"/>
       <c r="I53" s="29"/>
       <c r="J53" s="35"/>
       <c r="K53" s="29"/>
@@ -5205,22 +5205,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:M48"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="K3:M3"/>
     <mergeCell ref="D49:I50"/>
     <mergeCell ref="K49:M50"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="F52:H53"/>
     <mergeCell ref="A49:C50"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="M38:M48"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5257,73 +5257,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="94" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="92" t="s">
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5331,12 +5331,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="91" t="s">
+      <c r="L4" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="91"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -6440,14 +6440,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="84" t="s">
+      <c r="I44" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="85"/>
+      <c r="J44" s="90"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="84"/>
-      <c r="N44" s="84"/>
+      <c r="M44" s="89"/>
+      <c r="N44" s="89"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6465,13 +6465,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="84"/>
-      <c r="J45" s="84"/>
-      <c r="K45" s="84"/>
-      <c r="L45" s="84"/>
-      <c r="M45" s="84"/>
-      <c r="N45" s="84"/>
-      <c r="O45" s="84"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
+      <c r="L45" s="89"/>
+      <c r="M45" s="89"/>
+      <c r="N45" s="89"/>
+      <c r="O45" s="89"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
@@ -6488,15 +6488,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="86" t="s">
+      <c r="I46" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="86"/>
-      <c r="K46" s="86"/>
-      <c r="L46" s="86"/>
-      <c r="M46" s="86"/>
-      <c r="N46" s="86"/>
-      <c r="O46" s="87"/>
+      <c r="J46" s="91"/>
+      <c r="K46" s="91"/>
+      <c r="L46" s="91"/>
+      <c r="M46" s="91"/>
+      <c r="N46" s="91"/>
+      <c r="O46" s="92"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
@@ -6519,13 +6519,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="84" t="s">
+      <c r="K47" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="84"/>
-      <c r="M47" s="84"/>
-      <c r="N47" s="84"/>
-      <c r="O47" s="88"/>
+      <c r="L47" s="89"/>
+      <c r="M47" s="89"/>
+      <c r="N47" s="89"/>
+      <c r="O47" s="93"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
@@ -6550,7 +6550,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="88"/>
+      <c r="O48" s="93"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -6575,7 +6575,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="88"/>
+      <c r="O49" s="93"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -6600,7 +6600,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="88"/>
+      <c r="O50" s="93"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -6625,7 +6625,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="88"/>
+      <c r="O51" s="93"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -6650,7 +6650,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="88"/>
+      <c r="O52" s="93"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -6675,7 +6675,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="88"/>
+      <c r="O53" s="93"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -6700,7 +6700,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="88"/>
+      <c r="O54" s="93"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
@@ -6725,7 +6725,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="88"/>
+      <c r="O55" s="93"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -6750,7 +6750,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="89"/>
+      <c r="O56" s="94"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
@@ -6770,49 +6770,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="80" t="s">
+      <c r="A58" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="80"/>
-      <c r="C58" s="80"/>
+      <c r="B58" s="95"/>
+      <c r="C58" s="95"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="83" t="s">
+      <c r="F58" s="98" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="83"/>
-      <c r="H58" s="83"/>
-      <c r="I58" s="83"/>
-      <c r="J58" s="83"/>
-      <c r="K58" s="83"/>
+      <c r="G58" s="98"/>
+      <c r="H58" s="98"/>
+      <c r="I58" s="98"/>
+      <c r="J58" s="98"/>
+      <c r="K58" s="98"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="81" t="s">
+      <c r="N58" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="81"/>
+      <c r="O58" s="96"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="82"/>
-      <c r="B59" s="82"/>
-      <c r="C59" s="82"/>
+      <c r="A59" s="97"/>
+      <c r="B59" s="97"/>
+      <c r="C59" s="97"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="83"/>
-      <c r="G59" s="83"/>
-      <c r="H59" s="83"/>
-      <c r="I59" s="83"/>
-      <c r="J59" s="83"/>
-      <c r="K59" s="83"/>
+      <c r="F59" s="98"/>
+      <c r="G59" s="98"/>
+      <c r="H59" s="98"/>
+      <c r="I59" s="98"/>
+      <c r="J59" s="98"/>
+      <c r="K59" s="98"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="82"/>
-      <c r="O59" s="82"/>
+      <c r="N59" s="97"/>
+      <c r="O59" s="97"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="82"/>
-      <c r="B60" s="82"/>
-      <c r="C60" s="82"/>
+      <c r="A60" s="97"/>
+      <c r="B60" s="97"/>
+      <c r="C60" s="97"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -6823,15 +6823,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="82"/>
-      <c r="O60" s="82"/>
+      <c r="N60" s="97"/>
+      <c r="O60" s="97"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="80" t="s">
+      <c r="A61" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="80"/>
-      <c r="C61" s="80"/>
+      <c r="B61" s="95"/>
+      <c r="C61" s="95"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -6842,11 +6842,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="81"/>
-      <c r="O61" s="81"/>
+      <c r="N61" s="96"/>
+      <c r="O61" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="A59:C60"/>
+    <mergeCell ref="N59:O60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="F58:K59"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A1:E1"/>
@@ -6854,19 +6867,6 @@
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="A59:C60"/>
-    <mergeCell ref="N59:O60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="F58:K59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
07.11.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/Others/Allocation Sheet 2.xlsx
+++ b/Others/Allocation Sheet 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068455B1-5C24-427D-9476-2E3DA23285CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2D89DE-1306-45B9-B21A-23655E592E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allocation Sheet" sheetId="3" r:id="rId1"/>
@@ -445,7 +445,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Md Muradur Rahman</t>
+    <t>Md Haider Khan</t>
   </si>
 </sst>
 </file>
@@ -931,9 +931,72 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -952,68 +1015,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1035,36 +1065,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4011,8 +4011,8 @@
   </sheetPr>
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4034,45 +4034,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
     </row>
     <row r="3" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="81"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
@@ -4082,11 +4082,11 @@
       <c r="J3" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
@@ -4864,13 +4864,13 @@
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
-      <c r="H36" s="54" t="s">
+      <c r="H36" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="54"/>
+      <c r="I36" s="73"/>
       <c r="J36" s="38"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="73"/>
       <c r="M36" s="41"/>
     </row>
     <row r="37" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4885,12 +4885,12 @@
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="54"/>
-      <c r="M37" s="54"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
     </row>
     <row r="38" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="45" t="s">
@@ -4904,14 +4904,14 @@
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
-      <c r="H38" s="55" t="s">
+      <c r="H38" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="56"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="77"/>
     </row>
     <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
@@ -4931,10 +4931,10 @@
       <c r="I39" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="54"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="54"/>
-      <c r="M39" s="57"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="73"/>
+      <c r="M39" s="78"/>
     </row>
     <row r="40" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="45" t="s">
@@ -4955,7 +4955,7 @@
       <c r="J40" s="38"/>
       <c r="K40" s="38"/>
       <c r="L40" s="38"/>
-      <c r="M40" s="57"/>
+      <c r="M40" s="78"/>
     </row>
     <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="45" t="s">
@@ -4976,7 +4976,7 @@
       <c r="J41" s="38"/>
       <c r="K41" s="38"/>
       <c r="L41" s="38"/>
-      <c r="M41" s="57"/>
+      <c r="M41" s="78"/>
     </row>
     <row r="42" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="45" t="s">
@@ -4997,7 +4997,7 @@
       <c r="J42" s="38"/>
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
-      <c r="M42" s="57"/>
+      <c r="M42" s="78"/>
     </row>
     <row r="43" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="45" t="s">
@@ -5018,7 +5018,7 @@
       <c r="J43" s="38"/>
       <c r="K43" s="38"/>
       <c r="L43" s="38"/>
-      <c r="M43" s="57"/>
+      <c r="M43" s="78"/>
     </row>
     <row r="44" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
@@ -5039,7 +5039,7 @@
       <c r="J44" s="38"/>
       <c r="K44" s="38"/>
       <c r="L44" s="38"/>
-      <c r="M44" s="57"/>
+      <c r="M44" s="78"/>
     </row>
     <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="45" t="s">
@@ -5060,7 +5060,7 @@
       <c r="J45" s="38"/>
       <c r="K45" s="38"/>
       <c r="L45" s="38"/>
-      <c r="M45" s="57"/>
+      <c r="M45" s="78"/>
     </row>
     <row r="46" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="45"/>
@@ -5077,7 +5077,7 @@
       <c r="J46" s="38"/>
       <c r="K46" s="38"/>
       <c r="L46" s="38"/>
-      <c r="M46" s="57"/>
+      <c r="M46" s="78"/>
     </row>
     <row r="47" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="45"/>
@@ -5094,7 +5094,7 @@
       <c r="J47" s="38"/>
       <c r="K47" s="38"/>
       <c r="L47" s="38"/>
-      <c r="M47" s="57"/>
+      <c r="M47" s="78"/>
     </row>
     <row r="48" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="44"/>
@@ -5111,43 +5111,43 @@
       <c r="J48" s="38"/>
       <c r="K48" s="38"/>
       <c r="L48" s="38"/>
-      <c r="M48" s="58"/>
+      <c r="M48" s="79"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="78" t="s">
+      <c r="A49" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="79"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="64" t="s">
+      <c r="B49" s="69"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="64"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
       <c r="J49" s="32"/>
-      <c r="K49" s="66" t="s">
+      <c r="K49" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="L49" s="66"/>
-      <c r="M49" s="67"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="57"/>
     </row>
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="80"/>
-      <c r="B50" s="81"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="65"/>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="65"/>
-      <c r="I50" s="65"/>
+      <c r="A50" s="70"/>
+      <c r="B50" s="71"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="55"/>
+      <c r="I50" s="55"/>
       <c r="J50" s="33"/>
-      <c r="K50" s="68"/>
-      <c r="L50" s="68"/>
-      <c r="M50" s="69"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="59"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="29"/>
@@ -5165,25 +5165,25 @@
       <c r="M51" s="30"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="70" t="s">
+      <c r="A52" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="70"/>
+      <c r="B52" s="60"/>
       <c r="C52" s="35"/>
       <c r="D52" s="29"/>
       <c r="E52" s="29"/>
-      <c r="F52" s="72" t="s">
+      <c r="F52" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="G52" s="73"/>
-      <c r="H52" s="74"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="64"/>
       <c r="I52" s="29"/>
       <c r="J52" s="35"/>
-      <c r="K52" s="71" t="s">
+      <c r="K52" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="L52" s="71"/>
-      <c r="M52" s="71"/>
+      <c r="L52" s="61"/>
+      <c r="M52" s="61"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="34"/>
@@ -5191,9 +5191,9 @@
       <c r="C53" s="35"/>
       <c r="D53" s="29"/>
       <c r="E53" s="29"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="76"/>
-      <c r="H53" s="77"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="66"/>
+      <c r="H53" s="67"/>
       <c r="I53" s="29"/>
       <c r="J53" s="35"/>
       <c r="K53" s="29"/>
@@ -5205,22 +5205,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="M38:M48"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="D49:I50"/>
     <mergeCell ref="K49:M50"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="F52:H53"/>
     <mergeCell ref="A49:C50"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:M48"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5257,73 +5257,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="96" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="84" t="s">
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5331,12 +5331,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="83" t="s">
+      <c r="L4" s="93" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="93"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -6440,14 +6440,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="89" t="s">
+      <c r="I44" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="90"/>
+      <c r="J44" s="87"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="89"/>
-      <c r="N44" s="89"/>
+      <c r="M44" s="86"/>
+      <c r="N44" s="86"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6465,13 +6465,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="89"/>
-      <c r="K45" s="89"/>
-      <c r="L45" s="89"/>
-      <c r="M45" s="89"/>
-      <c r="N45" s="89"/>
-      <c r="O45" s="89"/>
+      <c r="I45" s="86"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="86"/>
+      <c r="L45" s="86"/>
+      <c r="M45" s="86"/>
+      <c r="N45" s="86"/>
+      <c r="O45" s="86"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
@@ -6488,15 +6488,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="91" t="s">
+      <c r="I46" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="91"/>
-      <c r="K46" s="91"/>
-      <c r="L46" s="91"/>
-      <c r="M46" s="91"/>
-      <c r="N46" s="91"/>
-      <c r="O46" s="92"/>
+      <c r="J46" s="88"/>
+      <c r="K46" s="88"/>
+      <c r="L46" s="88"/>
+      <c r="M46" s="88"/>
+      <c r="N46" s="88"/>
+      <c r="O46" s="89"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
@@ -6519,13 +6519,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="89" t="s">
+      <c r="K47" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="89"/>
-      <c r="M47" s="89"/>
-      <c r="N47" s="89"/>
-      <c r="O47" s="93"/>
+      <c r="L47" s="86"/>
+      <c r="M47" s="86"/>
+      <c r="N47" s="86"/>
+      <c r="O47" s="90"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
@@ -6550,7 +6550,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="93"/>
+      <c r="O48" s="90"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -6575,7 +6575,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="93"/>
+      <c r="O49" s="90"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -6600,7 +6600,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="93"/>
+      <c r="O50" s="90"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -6625,7 +6625,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="93"/>
+      <c r="O51" s="90"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -6650,7 +6650,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="93"/>
+      <c r="O52" s="90"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -6675,7 +6675,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="93"/>
+      <c r="O53" s="90"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -6700,7 +6700,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="93"/>
+      <c r="O54" s="90"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
@@ -6725,7 +6725,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="93"/>
+      <c r="O55" s="90"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -6750,7 +6750,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="94"/>
+      <c r="O56" s="91"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
@@ -6770,49 +6770,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="95" t="s">
+      <c r="A58" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="95"/>
-      <c r="C58" s="95"/>
+      <c r="B58" s="82"/>
+      <c r="C58" s="82"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="98" t="s">
+      <c r="F58" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="98"/>
-      <c r="H58" s="98"/>
-      <c r="I58" s="98"/>
-      <c r="J58" s="98"/>
-      <c r="K58" s="98"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="85"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="96" t="s">
+      <c r="N58" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="96"/>
+      <c r="O58" s="83"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="97"/>
-      <c r="B59" s="97"/>
-      <c r="C59" s="97"/>
+      <c r="A59" s="84"/>
+      <c r="B59" s="84"/>
+      <c r="C59" s="84"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="98"/>
-      <c r="G59" s="98"/>
-      <c r="H59" s="98"/>
-      <c r="I59" s="98"/>
-      <c r="J59" s="98"/>
-      <c r="K59" s="98"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="85"/>
+      <c r="J59" s="85"/>
+      <c r="K59" s="85"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="97"/>
-      <c r="O59" s="97"/>
+      <c r="N59" s="84"/>
+      <c r="O59" s="84"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="97"/>
-      <c r="B60" s="97"/>
-      <c r="C60" s="97"/>
+      <c r="A60" s="84"/>
+      <c r="B60" s="84"/>
+      <c r="C60" s="84"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -6823,15 +6823,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="97"/>
-      <c r="O60" s="97"/>
+      <c r="N60" s="84"/>
+      <c r="O60" s="84"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="95" t="s">
+      <c r="A61" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="95"/>
-      <c r="C61" s="95"/>
+      <c r="B61" s="82"/>
+      <c r="C61" s="82"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -6842,11 +6842,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="96"/>
-      <c r="O61" s="96"/>
+      <c r="N61" s="83"/>
+      <c r="O61" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="A59:C60"/>
@@ -6854,19 +6867,6 @@
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="F58:K59"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
09.11.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/Others/Allocation Sheet 2.xlsx
+++ b/Others/Allocation Sheet 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2D89DE-1306-45B9-B21A-23655E592E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDC8D43-23C4-4430-8AE9-FE1082188C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allocation Sheet" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="127">
   <si>
     <t>BL60</t>
   </si>
@@ -445,7 +445,10 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Md Haider Khan</t>
+    <t>Z20</t>
+  </si>
+  <si>
+    <t>Md Kamrul Islam</t>
   </si>
 </sst>
 </file>
@@ -931,6 +934,36 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -985,35 +1018,44 @@
     <xf numFmtId="49" fontId="11" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1026,45 +1068,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4011,7 +4014,7 @@
   </sheetPr>
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection sqref="A1:M53"/>
     </sheetView>
   </sheetViews>
@@ -4034,45 +4037,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
     </row>
     <row r="3" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="81"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
@@ -4082,11 +4085,11 @@
       <c r="J3" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="K3" s="75" t="s">
-        <v>125</v>
-      </c>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
+      <c r="K3" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
@@ -4845,7 +4848,9 @@
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
       <c r="G35" s="38"/>
-      <c r="H35" s="43"/>
+      <c r="H35" s="43" t="s">
+        <v>125</v>
+      </c>
       <c r="I35" s="39"/>
       <c r="J35" s="38"/>
       <c r="K35" s="38"/>
@@ -4864,13 +4869,13 @@
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
-      <c r="H36" s="73" t="s">
+      <c r="H36" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="73"/>
+      <c r="I36" s="54"/>
       <c r="J36" s="38"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
       <c r="M36" s="41"/>
     </row>
     <row r="37" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4885,12 +4890,12 @@
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
-      <c r="H37" s="73"/>
-      <c r="I37" s="73"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="73"/>
-      <c r="L37" s="73"/>
-      <c r="M37" s="73"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="54"/>
     </row>
     <row r="38" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="45" t="s">
@@ -4904,14 +4909,14 @@
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
-      <c r="H38" s="76" t="s">
+      <c r="H38" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="76"/>
-      <c r="J38" s="76"/>
-      <c r="K38" s="76"/>
-      <c r="L38" s="76"/>
-      <c r="M38" s="77"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="56"/>
     </row>
     <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
@@ -4931,10 +4936,10 @@
       <c r="I39" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="73"/>
-      <c r="K39" s="73"/>
-      <c r="L39" s="73"/>
-      <c r="M39" s="78"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="54"/>
+      <c r="L39" s="54"/>
+      <c r="M39" s="57"/>
     </row>
     <row r="40" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="45" t="s">
@@ -4955,7 +4960,7 @@
       <c r="J40" s="38"/>
       <c r="K40" s="38"/>
       <c r="L40" s="38"/>
-      <c r="M40" s="78"/>
+      <c r="M40" s="57"/>
     </row>
     <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="45" t="s">
@@ -4976,7 +4981,7 @@
       <c r="J41" s="38"/>
       <c r="K41" s="38"/>
       <c r="L41" s="38"/>
-      <c r="M41" s="78"/>
+      <c r="M41" s="57"/>
     </row>
     <row r="42" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="45" t="s">
@@ -4997,7 +5002,7 @@
       <c r="J42" s="38"/>
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
-      <c r="M42" s="78"/>
+      <c r="M42" s="57"/>
     </row>
     <row r="43" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="45" t="s">
@@ -5018,7 +5023,7 @@
       <c r="J43" s="38"/>
       <c r="K43" s="38"/>
       <c r="L43" s="38"/>
-      <c r="M43" s="78"/>
+      <c r="M43" s="57"/>
     </row>
     <row r="44" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
@@ -5039,7 +5044,7 @@
       <c r="J44" s="38"/>
       <c r="K44" s="38"/>
       <c r="L44" s="38"/>
-      <c r="M44" s="78"/>
+      <c r="M44" s="57"/>
     </row>
     <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="45" t="s">
@@ -5060,7 +5065,7 @@
       <c r="J45" s="38"/>
       <c r="K45" s="38"/>
       <c r="L45" s="38"/>
-      <c r="M45" s="78"/>
+      <c r="M45" s="57"/>
     </row>
     <row r="46" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="45"/>
@@ -5077,7 +5082,7 @@
       <c r="J46" s="38"/>
       <c r="K46" s="38"/>
       <c r="L46" s="38"/>
-      <c r="M46" s="78"/>
+      <c r="M46" s="57"/>
     </row>
     <row r="47" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="45"/>
@@ -5094,7 +5099,7 @@
       <c r="J47" s="38"/>
       <c r="K47" s="38"/>
       <c r="L47" s="38"/>
-      <c r="M47" s="78"/>
+      <c r="M47" s="57"/>
     </row>
     <row r="48" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="44"/>
@@ -5111,43 +5116,43 @@
       <c r="J48" s="38"/>
       <c r="K48" s="38"/>
       <c r="L48" s="38"/>
-      <c r="M48" s="79"/>
+      <c r="M48" s="58"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="68" t="s">
+      <c r="A49" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="69"/>
-      <c r="C49" s="69"/>
-      <c r="D49" s="54" t="s">
+      <c r="B49" s="79"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="E49" s="54"/>
-      <c r="F49" s="54"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="54"/>
-      <c r="I49" s="54"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
       <c r="J49" s="32"/>
-      <c r="K49" s="56" t="s">
+      <c r="K49" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="L49" s="56"/>
-      <c r="M49" s="57"/>
+      <c r="L49" s="66"/>
+      <c r="M49" s="67"/>
     </row>
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="70"/>
-      <c r="B50" s="71"/>
-      <c r="C50" s="71"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="55"/>
-      <c r="I50" s="55"/>
+      <c r="A50" s="80"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="65"/>
+      <c r="H50" s="65"/>
+      <c r="I50" s="65"/>
       <c r="J50" s="33"/>
-      <c r="K50" s="58"/>
-      <c r="L50" s="58"/>
-      <c r="M50" s="59"/>
+      <c r="K50" s="68"/>
+      <c r="L50" s="68"/>
+      <c r="M50" s="69"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="29"/>
@@ -5165,25 +5170,25 @@
       <c r="M51" s="30"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="60" t="s">
+      <c r="A52" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="60"/>
+      <c r="B52" s="70"/>
       <c r="C52" s="35"/>
       <c r="D52" s="29"/>
       <c r="E52" s="29"/>
-      <c r="F52" s="62" t="s">
+      <c r="F52" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="G52" s="63"/>
-      <c r="H52" s="64"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="74"/>
       <c r="I52" s="29"/>
       <c r="J52" s="35"/>
-      <c r="K52" s="61" t="s">
+      <c r="K52" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="L52" s="61"/>
-      <c r="M52" s="61"/>
+      <c r="L52" s="71"/>
+      <c r="M52" s="71"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="34"/>
@@ -5191,9 +5196,9 @@
       <c r="C53" s="35"/>
       <c r="D53" s="29"/>
       <c r="E53" s="29"/>
-      <c r="F53" s="65"/>
-      <c r="G53" s="66"/>
-      <c r="H53" s="67"/>
+      <c r="F53" s="75"/>
+      <c r="G53" s="76"/>
+      <c r="H53" s="77"/>
       <c r="I53" s="29"/>
       <c r="J53" s="35"/>
       <c r="K53" s="29"/>
@@ -5205,22 +5210,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:M48"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="K3:M3"/>
     <mergeCell ref="D49:I50"/>
     <mergeCell ref="K49:M50"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="F52:H53"/>
     <mergeCell ref="A49:C50"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="M38:M48"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5257,73 +5262,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="96" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="94" t="s">
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5331,12 +5336,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="93" t="s">
+      <c r="L4" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="93"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -6440,14 +6445,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="86" t="s">
+      <c r="I44" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="87"/>
+      <c r="J44" s="90"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="86"/>
-      <c r="N44" s="86"/>
+      <c r="M44" s="89"/>
+      <c r="N44" s="89"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6465,13 +6470,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="86"/>
-      <c r="J45" s="86"/>
-      <c r="K45" s="86"/>
-      <c r="L45" s="86"/>
-      <c r="M45" s="86"/>
-      <c r="N45" s="86"/>
-      <c r="O45" s="86"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
+      <c r="L45" s="89"/>
+      <c r="M45" s="89"/>
+      <c r="N45" s="89"/>
+      <c r="O45" s="89"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
@@ -6488,15 +6493,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="88" t="s">
+      <c r="I46" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="88"/>
-      <c r="K46" s="88"/>
-      <c r="L46" s="88"/>
-      <c r="M46" s="88"/>
-      <c r="N46" s="88"/>
-      <c r="O46" s="89"/>
+      <c r="J46" s="91"/>
+      <c r="K46" s="91"/>
+      <c r="L46" s="91"/>
+      <c r="M46" s="91"/>
+      <c r="N46" s="91"/>
+      <c r="O46" s="92"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
@@ -6519,13 +6524,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="86" t="s">
+      <c r="K47" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="86"/>
-      <c r="M47" s="86"/>
-      <c r="N47" s="86"/>
-      <c r="O47" s="90"/>
+      <c r="L47" s="89"/>
+      <c r="M47" s="89"/>
+      <c r="N47" s="89"/>
+      <c r="O47" s="93"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
@@ -6550,7 +6555,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="90"/>
+      <c r="O48" s="93"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -6575,7 +6580,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="90"/>
+      <c r="O49" s="93"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -6600,7 +6605,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="90"/>
+      <c r="O50" s="93"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -6625,7 +6630,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="90"/>
+      <c r="O51" s="93"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -6650,7 +6655,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="90"/>
+      <c r="O52" s="93"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -6675,7 +6680,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="90"/>
+      <c r="O53" s="93"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -6700,7 +6705,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="90"/>
+      <c r="O54" s="93"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
@@ -6725,7 +6730,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="90"/>
+      <c r="O55" s="93"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -6750,7 +6755,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="91"/>
+      <c r="O56" s="94"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
@@ -6770,49 +6775,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="82" t="s">
+      <c r="A58" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="82"/>
-      <c r="C58" s="82"/>
+      <c r="B58" s="95"/>
+      <c r="C58" s="95"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="85" t="s">
+      <c r="F58" s="98" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="85"/>
-      <c r="H58" s="85"/>
-      <c r="I58" s="85"/>
-      <c r="J58" s="85"/>
-      <c r="K58" s="85"/>
+      <c r="G58" s="98"/>
+      <c r="H58" s="98"/>
+      <c r="I58" s="98"/>
+      <c r="J58" s="98"/>
+      <c r="K58" s="98"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="83" t="s">
+      <c r="N58" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="83"/>
+      <c r="O58" s="96"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="84"/>
-      <c r="B59" s="84"/>
-      <c r="C59" s="84"/>
+      <c r="A59" s="97"/>
+      <c r="B59" s="97"/>
+      <c r="C59" s="97"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="85"/>
-      <c r="H59" s="85"/>
-      <c r="I59" s="85"/>
-      <c r="J59" s="85"/>
-      <c r="K59" s="85"/>
+      <c r="F59" s="98"/>
+      <c r="G59" s="98"/>
+      <c r="H59" s="98"/>
+      <c r="I59" s="98"/>
+      <c r="J59" s="98"/>
+      <c r="K59" s="98"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="84"/>
-      <c r="O59" s="84"/>
+      <c r="N59" s="97"/>
+      <c r="O59" s="97"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="84"/>
-      <c r="B60" s="84"/>
-      <c r="C60" s="84"/>
+      <c r="A60" s="97"/>
+      <c r="B60" s="97"/>
+      <c r="C60" s="97"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -6823,15 +6828,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="84"/>
-      <c r="O60" s="84"/>
+      <c r="N60" s="97"/>
+      <c r="O60" s="97"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="82" t="s">
+      <c r="A61" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="82"/>
-      <c r="C61" s="82"/>
+      <c r="B61" s="95"/>
+      <c r="C61" s="95"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -6842,11 +6847,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="83"/>
-      <c r="O61" s="83"/>
+      <c r="N61" s="96"/>
+      <c r="O61" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="A59:C60"/>
+    <mergeCell ref="N59:O60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="F58:K59"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A1:E1"/>
@@ -6854,19 +6872,6 @@
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="A59:C60"/>
-    <mergeCell ref="N59:O60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="F58:K59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
13.11.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/Others/Allocation Sheet 2.xlsx
+++ b/Others/Allocation Sheet 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDC8D43-23C4-4430-8AE9-FE1082188C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC16CA4-84AB-4782-B882-301DBC2F3B57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="129">
   <si>
     <t>BL60</t>
   </si>
@@ -449,6 +450,12 @@
   </si>
   <si>
     <t>Md Kamrul Islam</t>
+  </si>
+  <si>
+    <t>L250i</t>
+  </si>
+  <si>
+    <t>V105</t>
   </si>
 </sst>
 </file>
@@ -934,9 +941,72 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -955,68 +1025,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1038,36 +1075,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4014,8 +4021,8 @@
   </sheetPr>
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection sqref="A1:M53"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4037,45 +4044,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
     </row>
     <row r="3" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="81"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
@@ -4085,11 +4092,11 @@
       <c r="J3" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
@@ -4630,11 +4637,9 @@
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
       <c r="H26" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="I26" s="40">
-        <v>4280</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="I26" s="40"/>
       <c r="J26" s="38"/>
       <c r="K26" s="38"/>
       <c r="L26" s="38"/>
@@ -4657,10 +4662,10 @@
       <c r="F27" s="38"/>
       <c r="G27" s="38"/>
       <c r="H27" s="44" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="I27" s="39">
-        <v>5020</v>
+        <v>4280</v>
       </c>
       <c r="J27" s="38"/>
       <c r="K27" s="38"/>
@@ -4684,10 +4689,10 @@
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
       <c r="H28" s="43" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I28" s="39">
-        <v>5280</v>
+        <v>5020</v>
       </c>
       <c r="J28" s="38"/>
       <c r="K28" s="38"/>
@@ -4711,10 +4716,10 @@
       <c r="F29" s="38"/>
       <c r="G29" s="38"/>
       <c r="H29" s="43" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="I29" s="39">
-        <v>4550</v>
+        <v>5280</v>
       </c>
       <c r="J29" s="38"/>
       <c r="K29" s="38"/>
@@ -4734,10 +4739,10 @@
       <c r="F30" s="38"/>
       <c r="G30" s="38"/>
       <c r="H30" s="43" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="I30" s="39">
-        <v>5100</v>
+        <v>4550</v>
       </c>
       <c r="J30" s="38"/>
       <c r="K30" s="38"/>
@@ -4757,10 +4762,10 @@
       <c r="F31" s="38"/>
       <c r="G31" s="38"/>
       <c r="H31" s="43" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I31" s="39">
-        <v>5390</v>
+        <v>5100</v>
       </c>
       <c r="J31" s="38"/>
       <c r="K31" s="38"/>
@@ -4780,10 +4785,10 @@
       <c r="F32" s="38"/>
       <c r="G32" s="38"/>
       <c r="H32" s="45" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="I32" s="40">
-        <v>12090</v>
+        <v>5390</v>
       </c>
       <c r="J32" s="38"/>
       <c r="K32" s="38"/>
@@ -4803,10 +4808,10 @@
       <c r="F33" s="38"/>
       <c r="G33" s="38"/>
       <c r="H33" s="43" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I33" s="39">
-        <v>12240</v>
+        <v>12090</v>
       </c>
       <c r="J33" s="38"/>
       <c r="K33" s="38"/>
@@ -4869,13 +4874,13 @@
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
-      <c r="H36" s="54" t="s">
+      <c r="H36" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="54"/>
+      <c r="I36" s="73"/>
       <c r="J36" s="38"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="73"/>
       <c r="M36" s="41"/>
     </row>
     <row r="37" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4890,12 +4895,12 @@
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="54"/>
-      <c r="M37" s="54"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
     </row>
     <row r="38" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="45" t="s">
@@ -4909,14 +4914,14 @@
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
-      <c r="H38" s="55" t="s">
+      <c r="H38" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="56"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="77"/>
     </row>
     <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
@@ -4936,10 +4941,10 @@
       <c r="I39" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="54"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="54"/>
-      <c r="M39" s="57"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="73"/>
+      <c r="M39" s="78"/>
     </row>
     <row r="40" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="45" t="s">
@@ -4960,7 +4965,7 @@
       <c r="J40" s="38"/>
       <c r="K40" s="38"/>
       <c r="L40" s="38"/>
-      <c r="M40" s="57"/>
+      <c r="M40" s="78"/>
     </row>
     <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="45" t="s">
@@ -4981,15 +4986,13 @@
       <c r="J41" s="38"/>
       <c r="K41" s="38"/>
       <c r="L41" s="38"/>
-      <c r="M41" s="57"/>
+      <c r="M41" s="78"/>
     </row>
     <row r="42" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="B42" s="46">
-        <v>1190</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B42" s="46"/>
       <c r="C42" s="38"/>
       <c r="D42" s="38"/>
       <c r="E42" s="38"/>
@@ -5002,14 +5005,14 @@
       <c r="J42" s="38"/>
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
-      <c r="M42" s="57"/>
+      <c r="M42" s="78"/>
     </row>
     <row r="43" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="45" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B43" s="46">
-        <v>1100</v>
+        <v>1190</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="38"/>
@@ -5023,14 +5026,14 @@
       <c r="J43" s="38"/>
       <c r="K43" s="38"/>
       <c r="L43" s="38"/>
-      <c r="M43" s="57"/>
+      <c r="M43" s="78"/>
     </row>
     <row r="44" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="B44" s="36">
-        <v>1250</v>
+        <v>1100</v>
       </c>
       <c r="C44" s="38"/>
       <c r="D44" s="38"/>
@@ -5044,14 +5047,14 @@
       <c r="J44" s="38"/>
       <c r="K44" s="38"/>
       <c r="L44" s="38"/>
-      <c r="M44" s="57"/>
+      <c r="M44" s="78"/>
     </row>
     <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="45" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B45" s="38">
-        <v>1370</v>
+        <v>1250</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="38"/>
@@ -5065,11 +5068,15 @@
       <c r="J45" s="38"/>
       <c r="K45" s="38"/>
       <c r="L45" s="38"/>
-      <c r="M45" s="57"/>
+      <c r="M45" s="78"/>
     </row>
     <row r="46" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="45"/>
-      <c r="B46" s="38"/>
+      <c r="A46" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="38">
+        <v>1370</v>
+      </c>
       <c r="C46" s="38"/>
       <c r="D46" s="38"/>
       <c r="E46" s="38"/>
@@ -5082,7 +5089,7 @@
       <c r="J46" s="38"/>
       <c r="K46" s="38"/>
       <c r="L46" s="38"/>
-      <c r="M46" s="57"/>
+      <c r="M46" s="78"/>
     </row>
     <row r="47" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="45"/>
@@ -5099,7 +5106,7 @@
       <c r="J47" s="38"/>
       <c r="K47" s="38"/>
       <c r="L47" s="38"/>
-      <c r="M47" s="57"/>
+      <c r="M47" s="78"/>
     </row>
     <row r="48" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="44"/>
@@ -5116,43 +5123,43 @@
       <c r="J48" s="38"/>
       <c r="K48" s="38"/>
       <c r="L48" s="38"/>
-      <c r="M48" s="58"/>
+      <c r="M48" s="79"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="78" t="s">
+      <c r="A49" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="79"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="64" t="s">
+      <c r="B49" s="69"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="64"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
       <c r="J49" s="32"/>
-      <c r="K49" s="66" t="s">
+      <c r="K49" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="L49" s="66"/>
-      <c r="M49" s="67"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="57"/>
     </row>
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="80"/>
-      <c r="B50" s="81"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="65"/>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="65"/>
-      <c r="I50" s="65"/>
+      <c r="A50" s="70"/>
+      <c r="B50" s="71"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="55"/>
+      <c r="I50" s="55"/>
       <c r="J50" s="33"/>
-      <c r="K50" s="68"/>
-      <c r="L50" s="68"/>
-      <c r="M50" s="69"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="59"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="29"/>
@@ -5170,25 +5177,25 @@
       <c r="M51" s="30"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="70" t="s">
+      <c r="A52" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="70"/>
+      <c r="B52" s="60"/>
       <c r="C52" s="35"/>
       <c r="D52" s="29"/>
       <c r="E52" s="29"/>
-      <c r="F52" s="72" t="s">
+      <c r="F52" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="G52" s="73"/>
-      <c r="H52" s="74"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="64"/>
       <c r="I52" s="29"/>
       <c r="J52" s="35"/>
-      <c r="K52" s="71" t="s">
+      <c r="K52" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="L52" s="71"/>
-      <c r="M52" s="71"/>
+      <c r="L52" s="61"/>
+      <c r="M52" s="61"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="34"/>
@@ -5196,9 +5203,9 @@
       <c r="C53" s="35"/>
       <c r="D53" s="29"/>
       <c r="E53" s="29"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="76"/>
-      <c r="H53" s="77"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="66"/>
+      <c r="H53" s="67"/>
       <c r="I53" s="29"/>
       <c r="J53" s="35"/>
       <c r="K53" s="29"/>
@@ -5210,22 +5217,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="M38:M48"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="D49:I50"/>
     <mergeCell ref="K49:M50"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="F52:H53"/>
     <mergeCell ref="A49:C50"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:M48"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5262,73 +5269,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="96" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="84" t="s">
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5336,12 +5343,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="83" t="s">
+      <c r="L4" s="93" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="93"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -6445,14 +6452,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="89" t="s">
+      <c r="I44" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="90"/>
+      <c r="J44" s="87"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="89"/>
-      <c r="N44" s="89"/>
+      <c r="M44" s="86"/>
+      <c r="N44" s="86"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6470,13 +6477,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="89"/>
-      <c r="K45" s="89"/>
-      <c r="L45" s="89"/>
-      <c r="M45" s="89"/>
-      <c r="N45" s="89"/>
-      <c r="O45" s="89"/>
+      <c r="I45" s="86"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="86"/>
+      <c r="L45" s="86"/>
+      <c r="M45" s="86"/>
+      <c r="N45" s="86"/>
+      <c r="O45" s="86"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
@@ -6493,15 +6500,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="91" t="s">
+      <c r="I46" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="91"/>
-      <c r="K46" s="91"/>
-      <c r="L46" s="91"/>
-      <c r="M46" s="91"/>
-      <c r="N46" s="91"/>
-      <c r="O46" s="92"/>
+      <c r="J46" s="88"/>
+      <c r="K46" s="88"/>
+      <c r="L46" s="88"/>
+      <c r="M46" s="88"/>
+      <c r="N46" s="88"/>
+      <c r="O46" s="89"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
@@ -6524,13 +6531,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="89" t="s">
+      <c r="K47" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="89"/>
-      <c r="M47" s="89"/>
-      <c r="N47" s="89"/>
-      <c r="O47" s="93"/>
+      <c r="L47" s="86"/>
+      <c r="M47" s="86"/>
+      <c r="N47" s="86"/>
+      <c r="O47" s="90"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
@@ -6555,7 +6562,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="93"/>
+      <c r="O48" s="90"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -6580,7 +6587,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="93"/>
+      <c r="O49" s="90"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -6605,7 +6612,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="93"/>
+      <c r="O50" s="90"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -6630,7 +6637,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="93"/>
+      <c r="O51" s="90"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -6655,7 +6662,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="93"/>
+      <c r="O52" s="90"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -6680,7 +6687,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="93"/>
+      <c r="O53" s="90"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -6705,7 +6712,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="93"/>
+      <c r="O54" s="90"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
@@ -6730,7 +6737,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="93"/>
+      <c r="O55" s="90"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -6755,7 +6762,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="94"/>
+      <c r="O56" s="91"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
@@ -6775,49 +6782,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="95" t="s">
+      <c r="A58" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="95"/>
-      <c r="C58" s="95"/>
+      <c r="B58" s="82"/>
+      <c r="C58" s="82"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="98" t="s">
+      <c r="F58" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="98"/>
-      <c r="H58" s="98"/>
-      <c r="I58" s="98"/>
-      <c r="J58" s="98"/>
-      <c r="K58" s="98"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="85"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="96" t="s">
+      <c r="N58" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="96"/>
+      <c r="O58" s="83"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="97"/>
-      <c r="B59" s="97"/>
-      <c r="C59" s="97"/>
+      <c r="A59" s="84"/>
+      <c r="B59" s="84"/>
+      <c r="C59" s="84"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="98"/>
-      <c r="G59" s="98"/>
-      <c r="H59" s="98"/>
-      <c r="I59" s="98"/>
-      <c r="J59" s="98"/>
-      <c r="K59" s="98"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="85"/>
+      <c r="J59" s="85"/>
+      <c r="K59" s="85"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="97"/>
-      <c r="O59" s="97"/>
+      <c r="N59" s="84"/>
+      <c r="O59" s="84"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="97"/>
-      <c r="B60" s="97"/>
-      <c r="C60" s="97"/>
+      <c r="A60" s="84"/>
+      <c r="B60" s="84"/>
+      <c r="C60" s="84"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -6828,15 +6835,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="97"/>
-      <c r="O60" s="97"/>
+      <c r="N60" s="84"/>
+      <c r="O60" s="84"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="95" t="s">
+      <c r="A61" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="95"/>
-      <c r="C61" s="95"/>
+      <c r="B61" s="82"/>
+      <c r="C61" s="82"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -6847,11 +6854,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="96"/>
-      <c r="O61" s="96"/>
+      <c r="N61" s="83"/>
+      <c r="O61" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="A59:C60"/>
@@ -6859,19 +6879,6 @@
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="F58:K59"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
12.12.19 MC Sales Details
</commit_message>
<xml_diff>
--- a/Others/Allocation Sheet 2.xlsx
+++ b/Others/Allocation Sheet 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928B7109-19A9-4465-9584-3591ECE87FE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B813A29-18F4-4A8A-9BE3-2B430EC265AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,7 +461,7 @@
     </r>
   </si>
   <si>
-    <t>Md Haider Khan</t>
+    <t xml:space="preserve">Md Atikur Rahman </t>
   </si>
 </sst>
 </file>
@@ -904,14 +904,148 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -933,140 +1067,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3197,14 +3197,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>581026</xdr:colOff>
+      <xdr:colOff>409576</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -3236,7 +3236,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2447925" y="57150"/>
+          <a:off x="1733550" y="57150"/>
           <a:ext cx="485776" cy="371475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4014,7 +4014,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4036,59 +4036,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="70" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
     </row>
     <row r="3" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
       <c r="J3" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -4133,7 +4133,7 @@
       <c r="A5" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="62">
+      <c r="B5" s="40">
         <v>780</v>
       </c>
       <c r="C5" s="31"/>
@@ -4144,7 +4144,7 @@
       <c r="H5" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="63">
+      <c r="I5" s="41">
         <v>2780</v>
       </c>
       <c r="J5" s="31"/>
@@ -4156,7 +4156,7 @@
       <c r="A6" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="62">
+      <c r="B6" s="40">
         <v>810</v>
       </c>
       <c r="C6" s="31"/>
@@ -4167,7 +4167,7 @@
       <c r="H6" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="I6" s="63">
+      <c r="I6" s="41">
         <v>2770</v>
       </c>
       <c r="J6" s="31"/>
@@ -4179,7 +4179,7 @@
       <c r="A7" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="62">
+      <c r="B7" s="40">
         <v>800</v>
       </c>
       <c r="C7" s="31"/>
@@ -4190,7 +4190,7 @@
       <c r="H7" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="63">
+      <c r="I7" s="41">
         <v>6540</v>
       </c>
       <c r="J7" s="31"/>
@@ -4202,7 +4202,7 @@
       <c r="A8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="62">
+      <c r="B8" s="40">
         <v>790</v>
       </c>
       <c r="C8" s="31"/>
@@ -4213,7 +4213,7 @@
       <c r="H8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="63">
+      <c r="I8" s="41">
         <v>5290</v>
       </c>
       <c r="J8" s="31"/>
@@ -4225,7 +4225,7 @@
       <c r="A9" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="62">
+      <c r="B9" s="40">
         <v>800</v>
       </c>
       <c r="C9" s="31"/>
@@ -4236,7 +4236,7 @@
       <c r="H9" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="63">
+      <c r="I9" s="41">
         <v>5470</v>
       </c>
       <c r="J9" s="31"/>
@@ -4248,7 +4248,7 @@
       <c r="A10" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="62">
+      <c r="B10" s="40">
         <v>790</v>
       </c>
       <c r="C10" s="31"/>
@@ -4259,7 +4259,7 @@
       <c r="H10" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="63">
+      <c r="I10" s="41">
         <v>5750</v>
       </c>
       <c r="J10" s="31"/>
@@ -4271,7 +4271,7 @@
       <c r="A11" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="62">
+      <c r="B11" s="40">
         <v>800</v>
       </c>
       <c r="C11" s="31"/>
@@ -4282,7 +4282,7 @@
       <c r="H11" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="I11" s="63">
+      <c r="I11" s="41">
         <v>5550</v>
       </c>
       <c r="J11" s="31"/>
@@ -4294,7 +4294,7 @@
       <c r="A12" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="62">
+      <c r="B12" s="40">
         <v>915</v>
       </c>
       <c r="C12" s="31"/>
@@ -4305,7 +4305,7 @@
       <c r="H12" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="63">
+      <c r="I12" s="41">
         <v>5940</v>
       </c>
       <c r="J12" s="31"/>
@@ -4319,7 +4319,7 @@
       <c r="A13" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="62">
+      <c r="B13" s="40">
         <v>890</v>
       </c>
       <c r="C13" s="31"/>
@@ -4330,7 +4330,7 @@
       <c r="H13" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="63">
+      <c r="I13" s="41">
         <v>6530</v>
       </c>
       <c r="J13" s="31"/>
@@ -4342,7 +4342,7 @@
       <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="62">
+      <c r="B14" s="40">
         <v>920</v>
       </c>
       <c r="C14" s="31"/>
@@ -4353,7 +4353,7 @@
       <c r="H14" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="63">
+      <c r="I14" s="41">
         <v>6890</v>
       </c>
       <c r="J14" s="31"/>
@@ -4365,7 +4365,7 @@
       <c r="A15" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="62">
+      <c r="B15" s="40">
         <v>880</v>
       </c>
       <c r="C15" s="31"/>
@@ -4376,7 +4376,7 @@
       <c r="H15" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="I15" s="64">
+      <c r="I15" s="42">
         <v>8340</v>
       </c>
       <c r="J15" s="31"/>
@@ -4388,7 +4388,7 @@
       <c r="A16" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="62">
+      <c r="B16" s="40">
         <v>845</v>
       </c>
       <c r="C16" s="31"/>
@@ -4399,7 +4399,7 @@
       <c r="H16" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="64">
+      <c r="I16" s="42">
         <v>9190</v>
       </c>
       <c r="J16" s="31"/>
@@ -4411,7 +4411,7 @@
       <c r="A17" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="62">
+      <c r="B17" s="40">
         <v>970</v>
       </c>
       <c r="C17" s="31"/>
@@ -4422,7 +4422,7 @@
       <c r="H17" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="I17" s="64">
+      <c r="I17" s="42">
         <v>5750</v>
       </c>
       <c r="J17" s="31"/>
@@ -4434,7 +4434,7 @@
       <c r="A18" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="62">
+      <c r="B18" s="40">
         <v>1000</v>
       </c>
       <c r="C18" s="31"/>
@@ -4445,7 +4445,7 @@
       <c r="H18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="63">
+      <c r="I18" s="41">
         <v>3560</v>
       </c>
       <c r="J18" s="31"/>
@@ -4457,7 +4457,7 @@
       <c r="A19" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="62">
+      <c r="B19" s="40">
         <v>995</v>
       </c>
       <c r="C19" s="31"/>
@@ -4468,7 +4468,7 @@
       <c r="H19" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I19" s="63">
+      <c r="I19" s="41">
         <v>3340</v>
       </c>
       <c r="J19" s="31"/>
@@ -4480,7 +4480,7 @@
       <c r="A20" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="62">
+      <c r="B20" s="40">
         <v>880</v>
       </c>
       <c r="C20" s="31"/>
@@ -4491,7 +4491,7 @@
       <c r="H20" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="63">
+      <c r="I20" s="41">
         <v>4500</v>
       </c>
       <c r="J20" s="31"/>
@@ -4503,7 +4503,7 @@
       <c r="A21" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="62">
+      <c r="B21" s="40">
         <v>900</v>
       </c>
       <c r="C21" s="31"/>
@@ -4514,7 +4514,7 @@
       <c r="H21" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="63">
+      <c r="I21" s="41">
         <v>3710</v>
       </c>
       <c r="J21" s="31"/>
@@ -4526,7 +4526,7 @@
       <c r="A22" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="62">
+      <c r="B22" s="40">
         <v>1040</v>
       </c>
       <c r="C22" s="31"/>
@@ -4537,7 +4537,7 @@
       <c r="H22" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="64">
+      <c r="I22" s="42">
         <v>3620</v>
       </c>
       <c r="J22" s="31"/>
@@ -4549,7 +4549,7 @@
       <c r="A23" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="62">
+      <c r="B23" s="40">
         <v>1040</v>
       </c>
       <c r="C23" s="31"/>
@@ -4560,7 +4560,7 @@
       <c r="H23" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="I23" s="64">
+      <c r="I23" s="42">
         <v>4080</v>
       </c>
       <c r="J23" s="31"/>
@@ -4572,7 +4572,7 @@
       <c r="A24" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="62">
+      <c r="B24" s="40">
         <v>930</v>
       </c>
       <c r="C24" s="31"/>
@@ -4583,7 +4583,7 @@
       <c r="H24" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="I24" s="64">
+      <c r="I24" s="42">
         <v>4220</v>
       </c>
       <c r="J24" s="31"/>
@@ -4595,7 +4595,7 @@
       <c r="A25" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="62">
+      <c r="B25" s="40">
         <v>1190</v>
       </c>
       <c r="C25" s="31"/>
@@ -4606,7 +4606,7 @@
       <c r="H25" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="I25" s="63">
+      <c r="I25" s="41">
         <v>3710</v>
       </c>
       <c r="J25" s="31"/>
@@ -4622,7 +4622,7 @@
       <c r="A26" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="62">
+      <c r="B26" s="40">
         <v>1170</v>
       </c>
       <c r="C26" s="31"/>
@@ -4633,7 +4633,9 @@
       <c r="H26" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="I26" s="64"/>
+      <c r="I26" s="42">
+        <v>3890</v>
+      </c>
       <c r="J26" s="31"/>
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
@@ -4647,7 +4649,7 @@
       <c r="A27" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="62">
+      <c r="B27" s="40">
         <v>1190</v>
       </c>
       <c r="C27" s="31"/>
@@ -4658,7 +4660,7 @@
       <c r="H27" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="63">
+      <c r="I27" s="41">
         <v>4280</v>
       </c>
       <c r="J27" s="31"/>
@@ -4674,7 +4676,7 @@
       <c r="A28" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="62">
+      <c r="B28" s="40">
         <v>1080</v>
       </c>
       <c r="C28" s="31"/>
@@ -4685,7 +4687,7 @@
       <c r="H28" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="63">
+      <c r="I28" s="41">
         <v>5020</v>
       </c>
       <c r="J28" s="31"/>
@@ -4701,7 +4703,7 @@
       <c r="A29" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="62">
+      <c r="B29" s="40">
         <v>1100</v>
       </c>
       <c r="C29" s="31"/>
@@ -4712,7 +4714,7 @@
       <c r="H29" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I29" s="63">
+      <c r="I29" s="41">
         <v>5280</v>
       </c>
       <c r="J29" s="31"/>
@@ -4724,7 +4726,7 @@
       <c r="A30" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="62">
+      <c r="B30" s="40">
         <v>1010</v>
       </c>
       <c r="C30" s="31"/>
@@ -4735,7 +4737,7 @@
       <c r="H30" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="I30" s="63">
+      <c r="I30" s="41">
         <v>4550</v>
       </c>
       <c r="J30" s="31"/>
@@ -4747,7 +4749,7 @@
       <c r="A31" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="62">
+      <c r="B31" s="40">
         <v>1040</v>
       </c>
       <c r="C31" s="31"/>
@@ -4758,7 +4760,7 @@
       <c r="H31" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="I31" s="63">
+      <c r="I31" s="41">
         <v>5100</v>
       </c>
       <c r="J31" s="31"/>
@@ -4770,7 +4772,7 @@
       <c r="A32" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="B32" s="62">
+      <c r="B32" s="40">
         <v>970</v>
       </c>
       <c r="C32" s="31"/>
@@ -4781,7 +4783,7 @@
       <c r="H32" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="I32" s="64">
+      <c r="I32" s="42">
         <v>5390</v>
       </c>
       <c r="J32" s="31"/>
@@ -4793,7 +4795,7 @@
       <c r="A33" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="62">
+      <c r="B33" s="40">
         <v>1100</v>
       </c>
       <c r="C33" s="31"/>
@@ -4804,7 +4806,7 @@
       <c r="H33" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="I33" s="63">
+      <c r="I33" s="41">
         <v>12090</v>
       </c>
       <c r="J33" s="31"/>
@@ -4816,7 +4818,7 @@
       <c r="A34" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="62">
+      <c r="B34" s="40">
         <v>1050</v>
       </c>
       <c r="C34" s="31"/>
@@ -4827,7 +4829,7 @@
       <c r="H34" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="I34" s="63">
+      <c r="I34" s="41">
         <v>7890</v>
       </c>
       <c r="J34" s="31"/>
@@ -4839,7 +4841,7 @@
       <c r="A35" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="62">
+      <c r="B35" s="40">
         <v>1130</v>
       </c>
       <c r="C35" s="31"/>
@@ -4850,7 +4852,7 @@
       <c r="H35" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I35" s="63">
+      <c r="I35" s="41">
         <v>8310</v>
       </c>
       <c r="J35" s="31"/>
@@ -4862,7 +4864,7 @@
       <c r="A36" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="62" t="s">
+      <c r="B36" s="40" t="s">
         <v>127</v>
       </c>
       <c r="C36" s="31"/>
@@ -4870,20 +4872,20 @@
       <c r="E36" s="31"/>
       <c r="F36" s="31"/>
       <c r="G36" s="31"/>
-      <c r="H36" s="65" t="s">
+      <c r="H36" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="65"/>
+      <c r="I36" s="69"/>
       <c r="J36" s="31"/>
-      <c r="K36" s="65"/>
-      <c r="L36" s="65"/>
-      <c r="M36" s="66"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="69"/>
+      <c r="M36" s="43"/>
     </row>
     <row r="37" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="62">
+      <c r="B37" s="40">
         <v>1330</v>
       </c>
       <c r="C37" s="31"/>
@@ -4891,12 +4893,12 @@
       <c r="E37" s="31"/>
       <c r="F37" s="31"/>
       <c r="G37" s="31"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="K37" s="65"/>
-      <c r="L37" s="65"/>
-      <c r="M37" s="65"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="69"/>
     </row>
     <row r="38" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
@@ -4910,14 +4912,14 @@
       <c r="E38" s="31"/>
       <c r="F38" s="31"/>
       <c r="G38" s="31"/>
-      <c r="H38" s="67" t="s">
+      <c r="H38" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="67"/>
-      <c r="J38" s="67"/>
-      <c r="K38" s="67"/>
-      <c r="L38" s="67"/>
-      <c r="M38" s="68"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="72"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="72"/>
+      <c r="M38" s="73"/>
     </row>
     <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
@@ -4934,13 +4936,13 @@
       <c r="H39" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="I39" s="64" t="s">
+      <c r="I39" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="65"/>
-      <c r="K39" s="65"/>
-      <c r="L39" s="65"/>
-      <c r="M39" s="69"/>
+      <c r="J39" s="69"/>
+      <c r="K39" s="69"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="74"/>
     </row>
     <row r="40" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
@@ -4957,11 +4959,11 @@
       <c r="H40" s="31">
         <v>1000</v>
       </c>
-      <c r="I40" s="64"/>
+      <c r="I40" s="42"/>
       <c r="J40" s="31"/>
       <c r="K40" s="31"/>
       <c r="L40" s="31"/>
-      <c r="M40" s="69"/>
+      <c r="M40" s="74"/>
     </row>
     <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
@@ -4978,11 +4980,11 @@
       <c r="H41" s="31">
         <v>500</v>
       </c>
-      <c r="I41" s="64"/>
+      <c r="I41" s="42"/>
       <c r="J41" s="31"/>
       <c r="K41" s="31"/>
       <c r="L41" s="31"/>
-      <c r="M41" s="69"/>
+      <c r="M41" s="74"/>
     </row>
     <row r="42" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
@@ -4999,11 +5001,11 @@
       <c r="H42" s="31">
         <v>100</v>
       </c>
-      <c r="I42" s="64"/>
+      <c r="I42" s="42"/>
       <c r="J42" s="31"/>
       <c r="K42" s="31"/>
       <c r="L42" s="31"/>
-      <c r="M42" s="69"/>
+      <c r="M42" s="74"/>
     </row>
     <row r="43" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
@@ -5020,11 +5022,11 @@
       <c r="H43" s="31">
         <v>50</v>
       </c>
-      <c r="I43" s="64"/>
+      <c r="I43" s="42"/>
       <c r="J43" s="31"/>
       <c r="K43" s="31"/>
       <c r="L43" s="31"/>
-      <c r="M43" s="69"/>
+      <c r="M43" s="74"/>
     </row>
     <row r="44" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
@@ -5041,11 +5043,11 @@
       <c r="H44" s="31">
         <v>20</v>
       </c>
-      <c r="I44" s="64"/>
+      <c r="I44" s="42"/>
       <c r="J44" s="31"/>
       <c r="K44" s="31"/>
       <c r="L44" s="31"/>
-      <c r="M44" s="69"/>
+      <c r="M44" s="74"/>
     </row>
     <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
@@ -5062,11 +5064,11 @@
       <c r="H45" s="31">
         <v>10</v>
       </c>
-      <c r="I45" s="64"/>
+      <c r="I45" s="42"/>
       <c r="J45" s="31"/>
       <c r="K45" s="31"/>
       <c r="L45" s="31"/>
-      <c r="M45" s="69"/>
+      <c r="M45" s="74"/>
     </row>
     <row r="46" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
@@ -5083,11 +5085,11 @@
       <c r="H46" s="31">
         <v>5</v>
       </c>
-      <c r="I46" s="64"/>
+      <c r="I46" s="42"/>
       <c r="J46" s="31"/>
       <c r="K46" s="31"/>
       <c r="L46" s="31"/>
-      <c r="M46" s="69"/>
+      <c r="M46" s="74"/>
     </row>
     <row r="47" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
@@ -5100,11 +5102,11 @@
       <c r="H47" s="31">
         <v>2</v>
       </c>
-      <c r="I47" s="64"/>
+      <c r="I47" s="42"/>
       <c r="J47" s="31"/>
       <c r="K47" s="31"/>
       <c r="L47" s="31"/>
-      <c r="M47" s="69"/>
+      <c r="M47" s="74"/>
     </row>
     <row r="48" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
@@ -5112,125 +5114,125 @@
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
       <c r="E48" s="30"/>
-      <c r="F48" s="70"/>
-      <c r="G48" s="70"/>
-      <c r="H48" s="70" t="s">
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44" t="s">
         <v>12</v>
       </c>
       <c r="I48" s="31"/>
       <c r="J48" s="31"/>
       <c r="K48" s="31"/>
       <c r="L48" s="31"/>
-      <c r="M48" s="71"/>
+      <c r="M48" s="75"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="72" t="s">
+      <c r="A49" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
-      <c r="D49" s="74" t="s">
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="74"/>
-      <c r="I49" s="74"/>
-      <c r="J49" s="75"/>
-      <c r="K49" s="76" t="s">
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="L49" s="76"/>
-      <c r="M49" s="77"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="53"/>
     </row>
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="78"/>
-      <c r="B50" s="79"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="80"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="80"/>
-      <c r="G50" s="80"/>
-      <c r="H50" s="80"/>
-      <c r="I50" s="80"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="82"/>
-      <c r="L50" s="82"/>
-      <c r="M50" s="83"/>
+      <c r="A50" s="66"/>
+      <c r="B50" s="67"/>
+      <c r="C50" s="67"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="54"/>
+      <c r="L50" s="54"/>
+      <c r="M50" s="55"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="84"/>
-      <c r="B51" s="84"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
-      <c r="F51" s="84"/>
-      <c r="G51" s="84"/>
-      <c r="H51" s="84"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="47"/>
       <c r="I51" s="18"/>
       <c r="J51" s="18"/>
       <c r="K51" s="18"/>
-      <c r="L51" s="85"/>
-      <c r="M51" s="85"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="86" t="s">
+      <c r="A52" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="86"/>
+      <c r="B52" s="56"/>
       <c r="C52" s="17"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="87" t="s">
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="G52" s="88"/>
-      <c r="H52" s="89"/>
-      <c r="I52" s="84"/>
+      <c r="G52" s="59"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="47"/>
       <c r="J52" s="17"/>
-      <c r="K52" s="90" t="s">
+      <c r="K52" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="L52" s="90"/>
-      <c r="M52" s="90"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="57"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="91"/>
-      <c r="B53" s="91"/>
+      <c r="A53" s="49"/>
+      <c r="B53" s="49"/>
       <c r="C53" s="17"/>
-      <c r="D53" s="84"/>
-      <c r="E53" s="84"/>
-      <c r="F53" s="92"/>
-      <c r="G53" s="93"/>
-      <c r="H53" s="94"/>
-      <c r="I53" s="84"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="63"/>
+      <c r="I53" s="47"/>
       <c r="J53" s="17"/>
-      <c r="K53" s="84"/>
-      <c r="L53" s="84"/>
-      <c r="M53" s="84"/>
+      <c r="K53" s="47"/>
+      <c r="L53" s="47"/>
+      <c r="M53" s="47"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N57" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="M38:M48"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="D49:I50"/>
     <mergeCell ref="K49:M50"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="F52:H53"/>
     <mergeCell ref="A49:C50"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:M48"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5267,73 +5269,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="44" t="s">
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5341,12 +5343,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="43" t="s">
+      <c r="L4" s="89" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -6450,14 +6452,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="49" t="s">
+      <c r="I44" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="50"/>
+      <c r="J44" s="83"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="49"/>
+      <c r="M44" s="82"/>
+      <c r="N44" s="82"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6475,13 +6477,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="49"/>
-      <c r="K45" s="49"/>
-      <c r="L45" s="49"/>
-      <c r="M45" s="49"/>
-      <c r="N45" s="49"/>
-      <c r="O45" s="49"/>
+      <c r="I45" s="82"/>
+      <c r="J45" s="82"/>
+      <c r="K45" s="82"/>
+      <c r="L45" s="82"/>
+      <c r="M45" s="82"/>
+      <c r="N45" s="82"/>
+      <c r="O45" s="82"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
@@ -6498,15 +6500,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="51" t="s">
+      <c r="I46" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="51"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="51"/>
-      <c r="O46" s="52"/>
+      <c r="J46" s="84"/>
+      <c r="K46" s="84"/>
+      <c r="L46" s="84"/>
+      <c r="M46" s="84"/>
+      <c r="N46" s="84"/>
+      <c r="O46" s="85"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
@@ -6529,13 +6531,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="49" t="s">
+      <c r="K47" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="49"/>
-      <c r="M47" s="49"/>
-      <c r="N47" s="49"/>
-      <c r="O47" s="53"/>
+      <c r="L47" s="82"/>
+      <c r="M47" s="82"/>
+      <c r="N47" s="82"/>
+      <c r="O47" s="86"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
@@ -6560,7 +6562,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="53"/>
+      <c r="O48" s="86"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -6585,7 +6587,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="53"/>
+      <c r="O49" s="86"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -6610,7 +6612,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="53"/>
+      <c r="O50" s="86"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -6635,7 +6637,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="53"/>
+      <c r="O51" s="86"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -6660,7 +6662,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="53"/>
+      <c r="O52" s="86"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -6685,7 +6687,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="53"/>
+      <c r="O53" s="86"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -6710,7 +6712,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="53"/>
+      <c r="O54" s="86"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
@@ -6735,7 +6737,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="53"/>
+      <c r="O55" s="86"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -6760,7 +6762,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="54"/>
+      <c r="O56" s="87"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
@@ -6780,49 +6782,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="55"/>
-      <c r="C58" s="55"/>
+      <c r="B58" s="78"/>
+      <c r="C58" s="78"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="58" t="s">
+      <c r="F58" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="58"/>
-      <c r="J58" s="58"/>
-      <c r="K58" s="58"/>
+      <c r="G58" s="81"/>
+      <c r="H58" s="81"/>
+      <c r="I58" s="81"/>
+      <c r="J58" s="81"/>
+      <c r="K58" s="81"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="56" t="s">
+      <c r="N58" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="56"/>
+      <c r="O58" s="79"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="57"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="57"/>
+      <c r="A59" s="80"/>
+      <c r="B59" s="80"/>
+      <c r="C59" s="80"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
-      <c r="J59" s="58"/>
-      <c r="K59" s="58"/>
+      <c r="F59" s="81"/>
+      <c r="G59" s="81"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="81"/>
+      <c r="J59" s="81"/>
+      <c r="K59" s="81"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="57"/>
-      <c r="O59" s="57"/>
+      <c r="N59" s="80"/>
+      <c r="O59" s="80"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="57"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="57"/>
+      <c r="A60" s="80"/>
+      <c r="B60" s="80"/>
+      <c r="C60" s="80"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -6833,15 +6835,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="57"/>
-      <c r="O60" s="57"/>
+      <c r="N60" s="80"/>
+      <c r="O60" s="80"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="55" t="s">
+      <c r="A61" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="55"/>
-      <c r="C61" s="55"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="78"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -6852,11 +6854,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="56"/>
-      <c r="O61" s="56"/>
+      <c r="N61" s="79"/>
+      <c r="O61" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="A59:C60"/>
@@ -6864,19 +6879,6 @@
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="F58:K59"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
26.12.19 MC Sales Details
</commit_message>
<xml_diff>
--- a/Others/Allocation Sheet 2.xlsx
+++ b/Others/Allocation Sheet 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022C1485-F900-4A0D-BA85-5DD02570AAEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBAE13D-DA38-4972-A264-C27FD93124FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="135">
   <si>
     <t>BL60</t>
   </si>
@@ -410,6 +410,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Z25</t>
+  </si>
+  <si>
+    <t>BL98</t>
+  </si>
+  <si>
+    <t>i74</t>
+  </si>
+  <si>
+    <t>V102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Address: Rozy Market, Station Bazar, Natore</t>
   </si>
   <si>
     <r>
@@ -417,7 +432,6 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Berlin Sans FB Demi"/>
@@ -427,7 +441,6 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Berlin Sans FB Demi"/>
@@ -437,7 +450,6 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Berlin Sans FB Demi"/>
@@ -447,7 +459,6 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -458,22 +469,10 @@
     </r>
   </si>
   <si>
-    <t>Z25</t>
-  </si>
-  <si>
-    <t>BL98</t>
-  </si>
-  <si>
-    <t>i74</t>
-  </si>
-  <si>
-    <t>V102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         Address: Rozy Market, Station Bazar, Natore</t>
-  </si>
-  <si>
-    <t>Md Kamrul Islam</t>
+    <t>Md Haider Khan</t>
+  </si>
+  <si>
+    <t>Z12</t>
   </si>
 </sst>
 </file>
@@ -568,13 +567,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Berlin Sans FB Demi"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="13"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -588,40 +580,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="25"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Berlin Sans FB Demi"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Berlin Sans FB Demi"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -651,7 +642,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -737,32 +728,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -808,13 +773,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -882,202 +888,208 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4025,8 +4037,8 @@
   </sheetPr>
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4048,1199 +4060,1197 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+    </row>
+    <row r="3" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="94" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="93" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="91" t="s">
+        <v>133</v>
+      </c>
+      <c r="M3" s="92"/>
+    </row>
+    <row r="4" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="51"/>
+      <c r="H4" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="54">
+        <v>780</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="57">
+        <v>2780</v>
+      </c>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+    </row>
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="54">
+        <v>810</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="57">
+        <v>2770</v>
+      </c>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+    </row>
+    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="54">
+        <v>800</v>
+      </c>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="57">
+        <v>6540</v>
+      </c>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+    </row>
+    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="54">
+        <v>790</v>
+      </c>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="57">
+        <v>5290</v>
+      </c>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+    </row>
+    <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="54">
+        <v>800</v>
+      </c>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="57">
+        <v>5470</v>
+      </c>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+    </row>
+    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="54">
+        <v>790</v>
+      </c>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="57">
+        <v>5750</v>
+      </c>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+    </row>
+    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="54">
+        <v>800</v>
+      </c>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" s="57">
+        <v>5550</v>
+      </c>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+    </row>
+    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="54">
+        <v>915</v>
+      </c>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="57">
+        <v>5940</v>
+      </c>
+      <c r="J12" s="55"/>
+      <c r="K12" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+    </row>
+    <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="54">
+        <v>890</v>
+      </c>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13" s="57">
+        <v>5940</v>
+      </c>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="55"/>
+    </row>
+    <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="54">
+        <v>920</v>
+      </c>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="57">
+        <v>6530</v>
+      </c>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+    </row>
+    <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="54">
+        <v>880</v>
+      </c>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" s="58">
+        <v>6890</v>
+      </c>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+    </row>
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="54">
+        <v>845</v>
+      </c>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="58">
+        <v>5750</v>
+      </c>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+    </row>
+    <row r="17" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="58">
+        <v>3560</v>
+      </c>
+      <c r="J17" s="55"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="55"/>
+    </row>
+    <row r="18" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="54">
+        <v>970</v>
+      </c>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="57">
+        <v>3340</v>
+      </c>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="55"/>
+    </row>
+    <row r="19" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="54">
+        <v>1000</v>
+      </c>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="57">
+        <v>4500</v>
+      </c>
+      <c r="J19" s="55"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+    </row>
+    <row r="20" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="54">
+        <v>995</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="57">
+        <v>3710</v>
+      </c>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+    </row>
+    <row r="21" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="54">
+        <v>880</v>
+      </c>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="57">
+        <v>3620</v>
+      </c>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+    </row>
+    <row r="22" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="54">
+        <v>900</v>
+      </c>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="58">
+        <v>4080</v>
+      </c>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+    </row>
+    <row r="23" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="54">
+        <v>1040</v>
+      </c>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" s="58">
+        <v>4220</v>
+      </c>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+    </row>
+    <row r="24" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="54">
+        <v>1040</v>
+      </c>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" s="58">
+        <v>3710</v>
+      </c>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+    </row>
+    <row r="25" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="54">
+        <v>930</v>
+      </c>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="I25" s="57">
+        <v>3610</v>
+      </c>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="55"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="S25" s="27"/>
+    </row>
+    <row r="26" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="54">
+        <v>1190</v>
+      </c>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="I26" s="58">
+        <v>3890</v>
+      </c>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="27"/>
+    </row>
+    <row r="27" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="54">
+        <v>1170</v>
+      </c>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="57">
+        <v>4280</v>
+      </c>
+      <c r="J27" s="55"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="55"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="27"/>
+    </row>
+    <row r="28" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="54">
+        <v>1190</v>
+      </c>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="57">
+        <v>5020</v>
+      </c>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="27"/>
+      <c r="S28" s="27"/>
+    </row>
+    <row r="29" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="54">
+        <v>1080</v>
+      </c>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="I29" s="57">
+        <v>4550</v>
+      </c>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+    </row>
+    <row r="30" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="54">
+        <v>1100</v>
+      </c>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="57">
+        <v>5100</v>
+      </c>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="55"/>
+    </row>
+    <row r="31" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="54">
+        <v>1010</v>
+      </c>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" s="57">
+        <v>5390</v>
+      </c>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="55"/>
+    </row>
+    <row r="32" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="54">
+        <v>1040</v>
+      </c>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="I32" s="58"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="55"/>
+    </row>
+    <row r="33" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="54">
+        <v>970</v>
+      </c>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="I33" s="57">
+        <v>7890</v>
+      </c>
+      <c r="J33" s="55"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="55"/>
+    </row>
+    <row r="34" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="54">
+        <v>1100</v>
+      </c>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="57">
+        <v>8310</v>
+      </c>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="55"/>
+    </row>
+    <row r="35" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="54">
+        <v>1050</v>
+      </c>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-    </row>
-    <row r="3" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="K3" s="71" t="s">
-        <v>133</v>
-      </c>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-    </row>
-    <row r="4" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="36" t="s">
+      <c r="I35" s="57"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="55"/>
+    </row>
+    <row r="36" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="54">
+        <v>1130</v>
+      </c>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="60"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="61"/>
+    </row>
+    <row r="37" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
+    </row>
+    <row r="38" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="55">
+        <v>1330</v>
+      </c>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="62"/>
+      <c r="L38" s="62"/>
+      <c r="M38" s="63"/>
+    </row>
+    <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="55">
+        <v>1200</v>
+      </c>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="I39" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39" s="60"/>
+      <c r="K39" s="60"/>
+      <c r="L39" s="60"/>
+      <c r="M39" s="64"/>
+    </row>
+    <row r="40" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="55">
+        <v>1220</v>
+      </c>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55">
+        <v>1000</v>
+      </c>
+      <c r="I40" s="58"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="55"/>
+      <c r="M40" s="64"/>
+    </row>
+    <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="55">
+        <v>1070</v>
+      </c>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55">
+        <v>500</v>
+      </c>
+      <c r="I41" s="58"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="64"/>
+    </row>
+    <row r="42" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="55"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55">
+        <v>100</v>
+      </c>
+      <c r="I42" s="58"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="64"/>
+    </row>
+    <row r="43" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="55">
+        <v>1160</v>
+      </c>
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55">
+        <v>50</v>
+      </c>
+      <c r="I43" s="58"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="64"/>
+    </row>
+    <row r="44" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="53">
+        <v>1190</v>
+      </c>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55">
+        <v>20</v>
+      </c>
+      <c r="I44" s="58"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="64"/>
+    </row>
+    <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="55">
+        <v>1100</v>
+      </c>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55">
+        <v>10</v>
+      </c>
+      <c r="I45" s="58"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="55"/>
+      <c r="M45" s="64"/>
+    </row>
+    <row r="46" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="55">
+        <v>1250</v>
+      </c>
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55">
         <v>5</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="40">
-        <v>780</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" s="41">
-        <v>2780</v>
-      </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-    </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="40">
-        <v>810</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" s="41">
-        <v>2770</v>
-      </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-    </row>
-    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="40">
-        <v>800</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="I7" s="41">
-        <v>6540</v>
-      </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-    </row>
-    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="40">
-        <v>790</v>
-      </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="41">
-        <v>5290</v>
-      </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-    </row>
-    <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="40">
-        <v>800</v>
-      </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="41">
-        <v>5470</v>
-      </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-    </row>
-    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" s="40">
-        <v>790</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="41">
-        <v>5750</v>
-      </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-    </row>
-    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="40">
-        <v>800</v>
-      </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="I11" s="41">
-        <v>5550</v>
-      </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-    </row>
-    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="40">
-        <v>915</v>
-      </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="I12" s="41">
-        <v>5940</v>
-      </c>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-    </row>
-    <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="40">
-        <v>890</v>
-      </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="I13" s="41">
-        <v>5940</v>
-      </c>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-    </row>
-    <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+      <c r="I46" s="58"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="55"/>
+      <c r="L46" s="55"/>
+      <c r="M46" s="64"/>
+    </row>
+    <row r="47" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="55">
+        <v>1370</v>
+      </c>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="55">
         <v>2</v>
       </c>
-      <c r="B14" s="40">
-        <v>920</v>
-      </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="41">
-        <v>6530</v>
-      </c>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-    </row>
-    <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="40">
-        <v>880</v>
-      </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="I15" s="42">
-        <v>6890</v>
-      </c>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-    </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="40">
-        <v>845</v>
-      </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="42">
-        <v>9190</v>
-      </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-    </row>
-    <row r="17" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="I17" s="42">
-        <v>5750</v>
-      </c>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-    </row>
-    <row r="18" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="40">
-        <v>970</v>
-      </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="41">
-        <v>3560</v>
-      </c>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-    </row>
-    <row r="19" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="40">
-        <v>1000</v>
-      </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="I19" s="41">
-        <v>3340</v>
-      </c>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-    </row>
-    <row r="20" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="40">
-        <v>995</v>
-      </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="41">
-        <v>4500</v>
-      </c>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-    </row>
-    <row r="21" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="40">
-        <v>880</v>
-      </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="41">
-        <v>3710</v>
-      </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-    </row>
-    <row r="22" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="40">
-        <v>900</v>
-      </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="42">
-        <v>3620</v>
-      </c>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-    </row>
-    <row r="23" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="40">
-        <v>1040</v>
-      </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" s="42">
-        <v>4080</v>
-      </c>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-    </row>
-    <row r="24" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="40">
-        <v>1040</v>
-      </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="42">
-        <v>4220</v>
-      </c>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-    </row>
-    <row r="25" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="40">
-        <v>930</v>
-      </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="I25" s="41">
-        <v>3710</v>
-      </c>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-    </row>
-    <row r="26" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="40">
-        <v>1190</v>
-      </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="30" t="s">
+      <c r="I47" s="58"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="55"/>
+      <c r="L47" s="55"/>
+      <c r="M47" s="64"/>
+    </row>
+    <row r="48" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="53"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="65"/>
+      <c r="H48" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="55"/>
+      <c r="M48" s="66"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" s="68"/>
+      <c r="C49" s="68"/>
+      <c r="D49" s="69" t="s">
         <v>131</v>
       </c>
-      <c r="I26" s="42">
-        <v>3610</v>
-      </c>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="P26" s="32"/>
-      <c r="Q26" s="33"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="28"/>
-    </row>
-    <row r="27" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="40">
-        <v>1170</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="I27" s="41">
-        <v>3890</v>
-      </c>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="P27" s="32"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="28"/>
-    </row>
-    <row r="28" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="40">
-        <v>1190</v>
-      </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" s="41">
-        <v>4280</v>
-      </c>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="28"/>
-      <c r="S28" s="28"/>
-    </row>
-    <row r="29" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="40">
-        <v>1080</v>
-      </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="41">
-        <v>5020</v>
-      </c>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-    </row>
-    <row r="30" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="40">
-        <v>1100</v>
-      </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="I30" s="41">
-        <v>4550</v>
-      </c>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-    </row>
-    <row r="31" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="40">
-        <v>1010</v>
-      </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="41">
-        <v>5100</v>
-      </c>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-    </row>
-    <row r="32" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="40">
-        <v>1040</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I32" s="42">
-        <v>5390</v>
-      </c>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-    </row>
-    <row r="33" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="B33" s="40">
-        <v>970</v>
-      </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="I33" s="41">
-        <v>7890</v>
-      </c>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-    </row>
-    <row r="34" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="40">
-        <v>1100</v>
-      </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="I34" s="41">
-        <v>8310</v>
-      </c>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-    </row>
-    <row r="35" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="40">
-        <v>1050</v>
-      </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="I35" s="41"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-    </row>
-    <row r="36" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="40">
-        <v>1130</v>
-      </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="69"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="69"/>
-      <c r="L36" s="69"/>
-      <c r="M36" s="43"/>
-    </row>
-    <row r="37" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="69"/>
-      <c r="L37" s="69"/>
-      <c r="M37" s="69"/>
-    </row>
-    <row r="38" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="31">
-        <v>1330</v>
-      </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="73"/>
-    </row>
-    <row r="39" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="31">
-        <v>1200</v>
-      </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="I39" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="J39" s="69"/>
-      <c r="K39" s="69"/>
-      <c r="L39" s="69"/>
-      <c r="M39" s="74"/>
-    </row>
-    <row r="40" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="31">
-        <v>1220</v>
-      </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31">
-        <v>1000</v>
-      </c>
-      <c r="I40" s="42"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="74"/>
-    </row>
-    <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" s="31">
-        <v>1070</v>
-      </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31">
-        <v>500</v>
-      </c>
-      <c r="I41" s="42"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="74"/>
-    </row>
-    <row r="42" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31">
-        <v>100</v>
-      </c>
-      <c r="I42" s="42"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="74"/>
-    </row>
-    <row r="43" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" s="31">
-        <v>1160</v>
-      </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31">
-        <v>50</v>
-      </c>
-      <c r="I43" s="42"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="74"/>
-    </row>
-    <row r="44" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B44" s="30">
-        <v>1190</v>
-      </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31">
-        <v>20</v>
-      </c>
-      <c r="I44" s="42"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="31"/>
-      <c r="M44" s="74"/>
-    </row>
-    <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="B45" s="31">
-        <v>1100</v>
-      </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31">
-        <v>10</v>
-      </c>
-      <c r="I45" s="42"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
-      <c r="L45" s="31"/>
-      <c r="M45" s="74"/>
-    </row>
-    <row r="46" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="31">
-        <v>1250</v>
-      </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31">
-        <v>5</v>
-      </c>
-      <c r="I46" s="42"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="74"/>
-    </row>
-    <row r="47" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="31">
-        <v>1370</v>
-      </c>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31">
-        <v>2</v>
-      </c>
-      <c r="I47" s="42"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="74"/>
-    </row>
-    <row r="48" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="I48" s="31"/>
-      <c r="J48" s="31"/>
-      <c r="K48" s="31"/>
-      <c r="L48" s="31"/>
-      <c r="M48" s="75"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="50" t="s">
-        <v>132</v>
-      </c>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="52" t="s">
+      <c r="E49" s="69"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="69"/>
+      <c r="J49" s="70"/>
+      <c r="K49" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="L49" s="52"/>
-      <c r="M49" s="53"/>
+      <c r="L49" s="71"/>
+      <c r="M49" s="72"/>
     </row>
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="66"/>
-      <c r="B50" s="67"/>
-      <c r="C50" s="67"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="51"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="46"/>
-      <c r="K50" s="54"/>
-      <c r="L50" s="54"/>
-      <c r="M50" s="55"/>
+      <c r="A50" s="73"/>
+      <c r="B50" s="74"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="75"/>
+      <c r="I50" s="75"/>
+      <c r="J50" s="76"/>
+      <c r="K50" s="77"/>
+      <c r="L50" s="77"/>
+      <c r="M50" s="78"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
-      <c r="B51" s="47"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
+      <c r="A51" s="79"/>
+      <c r="B51" s="79"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="80"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="79"/>
+      <c r="H51" s="79"/>
+      <c r="I51" s="80"/>
+      <c r="J51" s="80"/>
+      <c r="K51" s="80"/>
+      <c r="L51" s="81"/>
+      <c r="M51" s="81"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="56"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="58" t="s">
+      <c r="B52" s="82"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="79"/>
+      <c r="E52" s="79"/>
+      <c r="F52" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="G52" s="59"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="47"/>
-      <c r="J52" s="17"/>
-      <c r="K52" s="57" t="s">
+      <c r="G52" s="84"/>
+      <c r="H52" s="85"/>
+      <c r="I52" s="79"/>
+      <c r="J52" s="27"/>
+      <c r="K52" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="L52" s="57"/>
-      <c r="M52" s="57"/>
+      <c r="L52" s="86"/>
+      <c r="M52" s="86"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="49"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="63"/>
-      <c r="I53" s="47"/>
-      <c r="J53" s="17"/>
-      <c r="K53" s="47"/>
-      <c r="L53" s="47"/>
-      <c r="M53" s="47"/>
+      <c r="A53" s="87"/>
+      <c r="B53" s="87"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="88"/>
+      <c r="G53" s="89"/>
+      <c r="H53" s="90"/>
+      <c r="I53" s="79"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="79"/>
+      <c r="L53" s="79"/>
+      <c r="M53" s="79"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N57" s="28"/>
+      <c r="N57" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:M48"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="K3:M3"/>
     <mergeCell ref="D49:I50"/>
     <mergeCell ref="K49:M50"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="F52:H53"/>
     <mergeCell ref="A49:C50"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="M38:M48"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5277,73 +5287,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="90" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5351,12 +5361,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="89" t="s">
+      <c r="L4" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -6460,14 +6470,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="82" t="s">
+      <c r="I44" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="83"/>
+      <c r="J44" s="38"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="82"/>
-      <c r="N44" s="82"/>
+      <c r="M44" s="37"/>
+      <c r="N44" s="37"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6485,13 +6495,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="82"/>
-      <c r="K45" s="82"/>
-      <c r="L45" s="82"/>
-      <c r="M45" s="82"/>
-      <c r="N45" s="82"/>
-      <c r="O45" s="82"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
+      <c r="O45" s="37"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
@@ -6508,15 +6518,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="84" t="s">
+      <c r="I46" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="84"/>
-      <c r="K46" s="84"/>
-      <c r="L46" s="84"/>
-      <c r="M46" s="84"/>
-      <c r="N46" s="84"/>
-      <c r="O46" s="85"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="39"/>
+      <c r="O46" s="40"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
@@ -6539,13 +6549,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="82" t="s">
+      <c r="K47" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="82"/>
-      <c r="M47" s="82"/>
-      <c r="N47" s="82"/>
-      <c r="O47" s="86"/>
+      <c r="L47" s="37"/>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37"/>
+      <c r="O47" s="41"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
@@ -6570,7 +6580,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="86"/>
+      <c r="O48" s="41"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -6595,7 +6605,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="86"/>
+      <c r="O49" s="41"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -6620,7 +6630,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="86"/>
+      <c r="O50" s="41"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -6645,7 +6655,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="86"/>
+      <c r="O51" s="41"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -6670,7 +6680,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="86"/>
+      <c r="O52" s="41"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -6695,7 +6705,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="86"/>
+      <c r="O53" s="41"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -6720,7 +6730,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="86"/>
+      <c r="O54" s="41"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
@@ -6745,7 +6755,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="86"/>
+      <c r="O55" s="41"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -6770,7 +6780,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="87"/>
+      <c r="O56" s="42"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
@@ -6790,49 +6800,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="78" t="s">
+      <c r="A58" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="78"/>
-      <c r="C58" s="78"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="81" t="s">
+      <c r="F58" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="81"/>
-      <c r="H58" s="81"/>
-      <c r="I58" s="81"/>
-      <c r="J58" s="81"/>
-      <c r="K58" s="81"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="46"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="79" t="s">
+      <c r="N58" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="79"/>
+      <c r="O58" s="44"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="80"/>
-      <c r="B59" s="80"/>
-      <c r="C59" s="80"/>
+      <c r="A59" s="45"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="81"/>
-      <c r="G59" s="81"/>
-      <c r="H59" s="81"/>
-      <c r="I59" s="81"/>
-      <c r="J59" s="81"/>
-      <c r="K59" s="81"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="46"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="80"/>
-      <c r="O59" s="80"/>
+      <c r="N59" s="45"/>
+      <c r="O59" s="45"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="80"/>
-      <c r="B60" s="80"/>
-      <c r="C60" s="80"/>
+      <c r="A60" s="45"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -6843,15 +6853,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="80"/>
-      <c r="O60" s="80"/>
+      <c r="N60" s="45"/>
+      <c r="O60" s="45"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="78" t="s">
+      <c r="A61" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="78"/>
-      <c r="C61" s="78"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -6862,11 +6872,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="79"/>
-      <c r="O61" s="79"/>
+      <c r="N61" s="44"/>
+      <c r="O61" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="A59:C60"/>
+    <mergeCell ref="N59:O60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="F58:K59"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A1:E1"/>
@@ -6874,19 +6897,6 @@
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="A59:C60"/>
-    <mergeCell ref="N59:O60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="F58:K59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>